<commit_message>
Refactors corrected offers generation
Simplifies the process of generating corrected offers by streamlining data merging and column renaming.
It ensures that the promotional price from the consolidated file is retained and renames columns for clarity.
Also updates the success message for better visibility.
</commit_message>
<xml_diff>
--- a/dados_produtos_corrigidos.xlsx
+++ b/dados_produtos_corrigidos.xlsx
@@ -462,163 +462,163 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>298239</v>
+        <v>258938</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>#01 MERCEARIA - ALTO GIRO</t>
+          <t>#01 MERCEARIA - #01 ALTO GIRO</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ACUCAR CRISTAL ECOCUCAR 2KG</t>
+          <t>ARROZ BRILHANTE TIPO1 BRANCO 5KG</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>AÇUCAR ECOÇUCAR CRISTAL  2KG</t>
+          <t>ARROZ BRILHANTE BRANCO TIPO 1 PCT 5KG</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>8.59</v>
+        <v>30.69</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>258938</v>
+        <v>269680</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>#01 MERCEARIA - ALTO GIRO</t>
+          <t>#01 MERCEARIA - #01 ALTO GIRO</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>ARROZ BRILHANTE TIPO1 BRANCO 5KG</t>
+          <t>ARROZ DONA VAVA 5KG TIPO 1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ARROZ BRILHANTE BRANCO TIPO 1 PCT 5KG</t>
+          <t>ARROZ DONA VAVA BRANCO TIPO 1 PCT 5KG</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>30.69</v>
+        <v>26.99</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>269680</v>
+        <v>136523</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>#01 MERCEARIA - ALTO GIRO</t>
+          <t>#01 MERCEARIA - #01 ALTO GIRO</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ARROZ DONA VAVA 5KG TIPO 1</t>
+          <t>ARROZ KOBLENZ TP1 BRANCO 5KG</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>ARROZ DONA VAVA BRANCO TIPO 1 PCT 5KG</t>
+          <t>ARROZ KOBLENZ BRANCO TIPO 1 PCT 5KG</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>26.99</v>
+        <v>30.99</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>136523</v>
+        <v>225003</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>#01 MERCEARIA - ALTO GIRO</t>
+          <t>#01 MERCEARIA - #01 ALTO GIRO</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ARROZ KOBLENZ TP1 BRANCO 5KG</t>
+          <t>ARROZ RAMPINELLI 5KG TIPO1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>ARROZ KOBLENZ BRANCO TIPO 1 PCT 5KG</t>
+          <t>ARROZ RAMPINELLI BRANCO TIPO 1 PCT 5KG</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>30.99</v>
+        <v>27.99</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>225003</v>
+        <v>100031</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>#01 MERCEARIA - ALTO GIRO</t>
+          <t>#01 MERCEARIA - #01 ALTO GIRO</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>ARROZ RAMPINELLI 5KG TIPO1</t>
+          <t>ARROZ REI  ARTHUR 5 KG BRANCO TIPO 1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>ARROZ RAMPINELLI BRANCO TIPO 1 PCT 5KG</t>
+          <t>ARROZ REI  ARTHUR BRANCO TIPO 1 PCT 5KG</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>27.99</v>
+        <v>31.99</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>100031</v>
+        <v>199440</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>#01 MERCEARIA - ALTO GIRO</t>
+          <t>#01 MERCEARIA - #01 ALTO GIRO</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ARROZ REI  ARTHUR 5 KG BRANCO TIPO 1</t>
+          <t>ARROZ SANTA FE 5 KG TP1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>ARROZ REI  ARTHUR BRANCO TIPO 1 PCT 5KG</t>
+          <t>ARROZ SANTA FE BRANCO TIPO 1 PCT 5KG</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>31.99</v>
+        <v>27.99</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>199440</v>
+        <v>298239</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>#01 MERCEARIA - ALTO GIRO</t>
+          <t>#01 MERCEARIA - #02 ALTO GIRO</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ARROZ SANTA FE 5 KG TP1</t>
+          <t>ACUCAR CRISTAL ECOCUCAR 2KG</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>ARROZ SANTA FE BRANCO TIPO 1 PCT 5KG</t>
+          <t>AÇUCAR ECOÇUCAR CRISTAL  2KG</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>27.99</v>
+        <v>8.59</v>
       </c>
     </row>
     <row r="9">
@@ -627,7 +627,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>#01 MERCEARIA - ALTO GIRO</t>
+          <t>#01 MERCEARIA - #02 ALTO GIRO</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -650,7 +650,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>#01 MERCEARIA - ALTO GIRO</t>
+          <t>#01 MERCEARIA - #02 ALTO GIRO</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">

</xml_diff>

<commit_message>
Updates data files with recent changes.
Refreshes data files to incorporate the latest updates and modifications, ensuring the accuracy and currency of the information used by the application.
</commit_message>
<xml_diff>
--- a/dados_produtos_corrigidos.xlsx
+++ b/dados_produtos_corrigidos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E508"/>
+  <dimension ref="A1:E510"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11265,6 +11265,52 @@
         <v>12.99</v>
       </c>
     </row>
+    <row r="509">
+      <c r="A509" t="n">
+        <v>142863</v>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>#03 LIMPEZA</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>DESINFETANTE BAK YPE 2L LAVANDA</t>
+        </is>
+      </c>
+      <c r="D509" t="inlineStr">
+        <is>
+          <t>DESINFETANTE YPE BAK 2L LAVANDA</t>
+        </is>
+      </c>
+      <c r="E509" t="n">
+        <v>12.99</v>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="n">
+        <v>148554</v>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>#03 LIMPEZA</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>DESINFETANTE BAK YPE EUCALIPTO 2LTS</t>
+        </is>
+      </c>
+      <c r="D510" t="inlineStr">
+        <is>
+          <t>DESINFETANTE YPE BAK 2L EUCALIPTO</t>
+        </is>
+      </c>
+      <c r="E510" t="n">
+        <v>12.99</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>